<commit_message>
Data Formate IN QBO
</commit_message>
<xml_diff>
--- a/server/data/coa/modifiedCoa.xlsx
+++ b/server/data/coa/modifiedCoa.xlsx
@@ -397,13 +397,1552 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E97"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Account No.</v>
+      </c>
+      <c r="B1" t="str">
+        <v>Account</v>
+      </c>
+      <c r="C1" t="str">
+        <v>Type</v>
+      </c>
+      <c r="D1" t="str">
+        <v>Detail type</v>
+      </c>
+      <c r="E1" t="str">
+        <v>Description</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2">
+        <v>2442</v>
+      </c>
+      <c r="B2" t="str">
+        <v>Australia and New Zealand Banking Group - ANZ (AU)</v>
+      </c>
+      <c r="C2" t="str">
+        <v>Cash and cash equivalents</v>
+      </c>
+      <c r="D2" t="str">
+        <v>Cash and cash equivalents</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3">
+        <v>2453</v>
+      </c>
+      <c r="B3" t="str">
+        <v>Cash and cash equivalents</v>
+      </c>
+      <c r="C3" t="str">
+        <v>Cash and cash equivalents</v>
+      </c>
+      <c r="D3" t="str">
+        <v>Cash and cash equivalents</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4">
+        <v>2454</v>
+      </c>
+      <c r="B4" t="str">
+        <v>Cash and cash equivalents:Cash and cash equivalents</v>
+      </c>
+      <c r="C4" t="str">
+        <v>Cash and cash equivalents</v>
+      </c>
+      <c r="D4" t="str">
+        <v>Cash and cash equivalents</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5">
+        <v>2480</v>
+      </c>
+      <c r="B5" t="str">
+        <v>Savings</v>
+      </c>
+      <c r="C5" t="str">
+        <v>Cash and cash equivalents</v>
+      </c>
+      <c r="D5" t="str">
+        <v>Cash and cash equivalents</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6">
+        <v>2482</v>
+      </c>
+      <c r="B6" t="str">
+        <v>Perm Staff Leave</v>
+      </c>
+      <c r="C6" t="str">
+        <v>Cash and cash equivalents</v>
+      </c>
+      <c r="D6" t="str">
+        <v>Cash and cash equivalents</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7">
+        <v>2483</v>
+      </c>
+      <c r="B7" t="str">
+        <v>Perm Staff Tax</v>
+      </c>
+      <c r="C7" t="str">
+        <v>Cash and cash equivalents</v>
+      </c>
+      <c r="D7" t="str">
+        <v>Cash and cash equivalents</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8">
+        <v>2484</v>
+      </c>
+      <c r="B8" t="str">
+        <v>Parramatta Council Bill</v>
+      </c>
+      <c r="C8" t="str">
+        <v>Cash and cash equivalents</v>
+      </c>
+      <c r="D8" t="str">
+        <v>Cash and cash equivalents</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9">
+        <v>2485</v>
+      </c>
+      <c r="B9" t="str">
+        <v>Cumberland Councill Bill</v>
+      </c>
+      <c r="C9" t="str">
+        <v>Cash and cash equivalents</v>
+      </c>
+      <c r="D9" t="str">
+        <v>Cash and cash equivalents</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10">
+        <v>2486</v>
+      </c>
+      <c r="B10" t="str">
+        <v>petty cash account</v>
+      </c>
+      <c r="C10" t="str">
+        <v>Cash and cash equivalents</v>
+      </c>
+      <c r="D10" t="str">
+        <v>Cash and cash equivalents</v>
+      </c>
+      <c r="E10" t="str">
+        <v>Petty Cash</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11">
+        <v>2487</v>
+      </c>
+      <c r="B11" t="str">
+        <v>Personal Savings Account</v>
+      </c>
+      <c r="C11" t="str">
+        <v>Cash and cash equivalents</v>
+      </c>
+      <c r="D11" t="str">
+        <v>Cash and cash equivalents</v>
+      </c>
+      <c r="E11" t="str">
+        <v>Personal Savings Account</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12">
+        <v>2488</v>
+      </c>
+      <c r="B12" t="str">
+        <v>KIA Cerrato expenses</v>
+      </c>
+      <c r="C12" t="str">
+        <v>Cash and cash equivalents</v>
+      </c>
+      <c r="D12" t="str">
+        <v>Cash and cash equivalents</v>
+      </c>
+      <c r="E12" t="str">
+        <v>KIA Cerrato expenses</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13">
+        <v>2489</v>
+      </c>
+      <c r="B13" t="str">
+        <v>BSS Savings Account</v>
+      </c>
+      <c r="C13" t="str">
+        <v>Cash and cash equivalents</v>
+      </c>
+      <c r="D13" t="str">
+        <v>Cash and cash equivalents</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14">
+        <v>2490</v>
+      </c>
+      <c r="B14" t="str">
+        <v>precision super payments</v>
+      </c>
+      <c r="C14" t="str">
+        <v>Cash and cash equivalents</v>
+      </c>
+      <c r="D14" t="str">
+        <v>Cash and cash equivalents</v>
+      </c>
+      <c r="E14" t="str">
+        <v>staff super payments</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15">
+        <v>2492</v>
+      </c>
+      <c r="B15" t="str">
+        <v>Learning &amp; Development</v>
+      </c>
+      <c r="C15" t="str">
+        <v>Cash and cash equivalents</v>
+      </c>
+      <c r="D15" t="str">
+        <v>Cash and cash equivalents</v>
+      </c>
+      <c r="E15" t="str">
+        <v>Learning &amp; Development</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16">
+        <v>2493</v>
+      </c>
+      <c r="B16" t="str">
+        <v>Saengdara SMSF</v>
+      </c>
+      <c r="C16" t="str">
+        <v>Cash and cash equivalents</v>
+      </c>
+      <c r="D16" t="str">
+        <v>Cash and cash equivalents</v>
+      </c>
+      <c r="E16" t="str">
+        <v>Saengdara SMSF</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17">
+        <v>2457</v>
+      </c>
+      <c r="B17" t="str">
+        <v>Accounts Receivable (A/R)</v>
+      </c>
+      <c r="C17" t="str">
+        <v>Accounts receivable (A/R)</v>
+      </c>
+      <c r="D17" t="str">
+        <v>Accounts receivable (A/R)</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18">
+        <v>2403</v>
+      </c>
+      <c r="B18" t="str">
+        <v>Uncategorised Asset</v>
+      </c>
+      <c r="C18" t="str">
+        <v>Current assets</v>
+      </c>
+      <c r="D18" t="str">
+        <v>Other current assets</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19">
+        <v>2428</v>
+      </c>
+      <c r="B19" t="str">
+        <v>Undeposited funds</v>
+      </c>
+      <c r="C19" t="str">
+        <v>Current assets</v>
+      </c>
+      <c r="D19" t="str">
+        <v>Other current assets</v>
+      </c>
+      <c r="E19" t="str">
+        <v>Money from the business not yet deposited into a business bank account</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20">
+        <v>2440</v>
+      </c>
+      <c r="B20" t="str">
+        <v>Inventory</v>
+      </c>
+      <c r="C20" t="str">
+        <v>Current assets</v>
+      </c>
+      <c r="D20" t="str">
+        <v>Other current assets</v>
+      </c>
+      <c r="E20" t="str">
+        <v>Inventory</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21">
+        <v>2451</v>
+      </c>
+      <c r="B21" t="str">
+        <v>Inventory Asset</v>
+      </c>
+      <c r="C21" t="str">
+        <v>Current assets</v>
+      </c>
+      <c r="D21" t="str">
+        <v>Other current assets</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22">
+        <v>2429</v>
+      </c>
+      <c r="B22" t="str">
+        <v>Motor vehicles at cost</v>
+      </c>
+      <c r="C22" t="str">
+        <v>Fixed assets</v>
+      </c>
+      <c r="D22" t="str">
+        <v>Other fixed assets</v>
+      </c>
+      <c r="E22" t="str">
+        <v>Cost of purchasing or leasing motor vehicles for business purposes</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23">
+        <v>2430</v>
+      </c>
+      <c r="B23" t="str">
+        <v>Office furniture and equipment at cost</v>
+      </c>
+      <c r="C23" t="str">
+        <v>Fixed assets</v>
+      </c>
+      <c r="D23" t="str">
+        <v>Other fixed assets</v>
+      </c>
+      <c r="E23" t="str">
+        <v>Cost of buying or leasing furniture and equipment</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24">
+        <v>2455</v>
+      </c>
+      <c r="B24" t="str">
+        <v>Accounts Payable (A/P)</v>
+      </c>
+      <c r="C24" t="str">
+        <v>Accounts payable (A/P)</v>
+      </c>
+      <c r="D24" t="str">
+        <v>Accounts Payable (A/P)</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25">
+        <v>2476</v>
+      </c>
+      <c r="B25" t="str">
+        <v>Workwear/Uniform</v>
+      </c>
+      <c r="C25" t="str">
+        <v>Credit card</v>
+      </c>
+      <c r="D25" t="str">
+        <v>Credit Card</v>
+      </c>
+      <c r="E25" t="str">
+        <v>Workwear/Uniform</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26">
+        <v>2477</v>
+      </c>
+      <c r="B26" t="str">
+        <v>Car Expense - VW</v>
+      </c>
+      <c r="C26" t="str">
+        <v>Credit card</v>
+      </c>
+      <c r="D26" t="str">
+        <v>Credit Card</v>
+      </c>
+      <c r="E26" t="str">
+        <v>Car Expense - VW</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27">
+        <v>2478</v>
+      </c>
+      <c r="B27" t="str">
+        <v>Credit Card Bankwest</v>
+      </c>
+      <c r="C27" t="str">
+        <v>Credit card</v>
+      </c>
+      <c r="D27" t="str">
+        <v>Credit Card</v>
+      </c>
+      <c r="E27" t="str">
+        <v>Expenses</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28">
+        <v>2479</v>
+      </c>
+      <c r="B28" t="str">
+        <v>ANZ Credit Card</v>
+      </c>
+      <c r="C28" t="str">
+        <v>Credit card</v>
+      </c>
+      <c r="D28" t="str">
+        <v>Credit Card</v>
+      </c>
+      <c r="E28" t="str">
+        <v>Expenses</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29">
+        <v>2481</v>
+      </c>
+      <c r="B29" t="str">
+        <v>Citibank Credit Card</v>
+      </c>
+      <c r="C29" t="str">
+        <v>Credit card</v>
+      </c>
+      <c r="D29" t="str">
+        <v>Credit Card</v>
+      </c>
+      <c r="E29" t="str">
+        <v>Citibank Credit Card</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30">
+        <v>2432</v>
+      </c>
+      <c r="B30" t="str">
+        <v>Payroll clearing</v>
+      </c>
+      <c r="C30" t="str">
+        <v>Current liabilities</v>
+      </c>
+      <c r="D30" t="str">
+        <v>Other current liabilities</v>
+      </c>
+      <c r="E30" t="str">
+        <v>An account used to deposit, record and monitor payrolls. No funds remain once all cheques clear</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31">
+        <v>2433</v>
+      </c>
+      <c r="B31" t="str">
+        <v>Superannuation - staff</v>
+      </c>
+      <c r="C31" t="str">
+        <v>Current liabilities</v>
+      </c>
+      <c r="D31" t="str">
+        <v>Other current liabilities</v>
+      </c>
+      <c r="E31" t="str">
+        <v>Superannuation expenses</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32">
+        <v>2436</v>
+      </c>
+      <c r="B32" t="str">
+        <v>Superannuation payable</v>
+      </c>
+      <c r="C32" t="str">
+        <v>Current liabilities</v>
+      </c>
+      <c r="D32" t="str">
+        <v>Other current liabilities</v>
+      </c>
+      <c r="E32" t="str">
+        <v>The amount of superannuation to be paid business to the superannuation fund(s) of employees</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33">
+        <v>2437</v>
+      </c>
+      <c r="B33" t="str">
+        <v>PAYG instalments payable</v>
+      </c>
+      <c r="C33" t="str">
+        <v>Current liabilities</v>
+      </c>
+      <c r="D33" t="str">
+        <v>Other current liabilities</v>
+      </c>
+      <c r="E33" t="str">
+        <v>Pay-As-You-Go instalments paid regularly to the ATO</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34">
+        <v>2446</v>
+      </c>
+      <c r="B34" t="str">
+        <v>PAYG Liability</v>
+      </c>
+      <c r="C34" t="str">
+        <v>Current liabilities</v>
+      </c>
+      <c r="D34" t="str">
+        <v>Other current liabilities</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35">
+        <v>2448</v>
+      </c>
+      <c r="B35" t="str">
+        <v>Default Liability</v>
+      </c>
+      <c r="C35" t="str">
+        <v>Current liabilities</v>
+      </c>
+      <c r="D35" t="str">
+        <v>Other current liabilities</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36">
+        <v>2461</v>
+      </c>
+      <c r="B36" t="str">
+        <v>ATO Clearing Account</v>
+      </c>
+      <c r="C36" t="str">
+        <v>Current liabilities</v>
+      </c>
+      <c r="D36" t="str">
+        <v>Other current liabilities</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37">
+        <v>2463</v>
+      </c>
+      <c r="B37" t="str">
+        <v>GST Liabilities Payable</v>
+      </c>
+      <c r="C37" t="str">
+        <v>Current liabilities</v>
+      </c>
+      <c r="D37" t="str">
+        <v>Other current liabilities</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38">
+        <v>2465</v>
+      </c>
+      <c r="B38" t="str">
+        <v>FBT Liabilities</v>
+      </c>
+      <c r="C38" t="str">
+        <v>Current liabilities</v>
+      </c>
+      <c r="D38" t="str">
+        <v>Other current liabilities</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39">
+        <v>2466</v>
+      </c>
+      <c r="B39" t="str">
+        <v>PAYG Instalment Liabilities</v>
+      </c>
+      <c r="C39" t="str">
+        <v>Current liabilities</v>
+      </c>
+      <c r="D39" t="str">
+        <v>Other current liabilities</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40">
+        <v>2467</v>
+      </c>
+      <c r="B40" t="str">
+        <v>Luxury Car Tax Liabilities</v>
+      </c>
+      <c r="C40" t="str">
+        <v>Current liabilities</v>
+      </c>
+      <c r="D40" t="str">
+        <v>Other current liabilities</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41">
+        <v>2468</v>
+      </c>
+      <c r="B41" t="str">
+        <v>WET Liabilities</v>
+      </c>
+      <c r="C41" t="str">
+        <v>Current liabilities</v>
+      </c>
+      <c r="D41" t="str">
+        <v>Other current liabilities</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42">
+        <v>2469</v>
+      </c>
+      <c r="B42" t="str">
+        <v>PAYG Withholdings Payable</v>
+      </c>
+      <c r="C42" t="str">
+        <v>Current liabilities</v>
+      </c>
+      <c r="D42" t="str">
+        <v>Other current liabilities</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43">
+        <v>2431</v>
+      </c>
+      <c r="B43" t="str">
+        <v>Loan</v>
+      </c>
+      <c r="C43" t="str">
+        <v>Non-current liabilities</v>
+      </c>
+      <c r="D43" t="str">
+        <v>Other non-current liabilities</v>
+      </c>
+      <c r="E43" t="str">
+        <v>Money borrowed for business purposes</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44">
+        <v>2491</v>
+      </c>
+      <c r="B44" t="str">
+        <v>Directors Loan</v>
+      </c>
+      <c r="C44" t="str">
+        <v>Non-current liabilities</v>
+      </c>
+      <c r="D44" t="str">
+        <v>Other non-current liabilities</v>
+      </c>
+      <c r="E44" t="str">
+        <v>Directors Loan</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45">
+        <v>2404</v>
+      </c>
+      <c r="B45" t="str">
+        <v>Retained Earnings</v>
+      </c>
+      <c r="C45" t="str">
+        <v>Owner's equity</v>
+      </c>
+      <c r="D45" t="str">
+        <v>Owner's Equity</v>
+      </c>
+      <c r="E45" t="str">
+        <v>Net earnings not paid out as dividends, but retained by the company to be reinvested</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46">
+        <v>2425</v>
+      </c>
+      <c r="B46" t="str">
+        <v>Opening balance equity</v>
+      </c>
+      <c r="C46" t="str">
+        <v>Owner's equity</v>
+      </c>
+      <c r="D46" t="str">
+        <v>Owner's Equity</v>
+      </c>
+      <c r="E46" t="str">
+        <v>Offsetting entry used when entering account balances in QuickBooks Online</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47">
+        <v>2426</v>
+      </c>
+      <c r="B47" t="str">
+        <v>Owners drawings</v>
+      </c>
+      <c r="C47" t="str">
+        <v>Owner's equity</v>
+      </c>
+      <c r="D47" t="str">
+        <v>Owner's Equity</v>
+      </c>
+      <c r="E47" t="str">
+        <v>Withdrawals from a company account to pay an owner</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48">
+        <v>2401</v>
+      </c>
+      <c r="B48" t="str">
+        <v>Uncategorised Income</v>
+      </c>
+      <c r="C48" t="str">
+        <v>Income</v>
+      </c>
+      <c r="D48" t="str">
+        <v>Revenue - General</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49">
+        <v>2441</v>
+      </c>
+      <c r="B49" t="str">
+        <v>Sales</v>
+      </c>
+      <c r="C49" t="str">
+        <v>Income</v>
+      </c>
+      <c r="D49" t="str">
+        <v>Revenue - General</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50">
+        <v>2443</v>
+      </c>
+      <c r="B50" t="str">
+        <v>Billable Expense Income</v>
+      </c>
+      <c r="C50" t="str">
+        <v>Income</v>
+      </c>
+      <c r="D50" t="str">
+        <v>Revenue - General</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51">
+        <v>2449</v>
+      </c>
+      <c r="B51" t="str">
+        <v>Sales of Product Income</v>
+      </c>
+      <c r="C51" t="str">
+        <v>Income</v>
+      </c>
+      <c r="D51" t="str">
+        <v>Revenue - General</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52">
+        <v>2458</v>
+      </c>
+      <c r="B52" t="str">
+        <v>Unapplied Cash Payment Income</v>
+      </c>
+      <c r="C52" t="str">
+        <v>Income</v>
+      </c>
+      <c r="D52" t="str">
+        <v>Revenue - General</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53">
+        <v>2438</v>
+      </c>
+      <c r="B53" t="str">
+        <v>Freight &amp; Delivery - COS</v>
+      </c>
+      <c r="C53" t="str">
+        <v>Cost of sales</v>
+      </c>
+      <c r="D53" t="str">
+        <v>Cost of Sales</v>
+      </c>
+      <c r="E53" t="str">
+        <v>Freight &amp; Delivery - COS</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54">
+        <v>2450</v>
+      </c>
+      <c r="B54" t="str">
+        <v>Cost of sales</v>
+      </c>
+      <c r="C54" t="str">
+        <v>Cost of sales</v>
+      </c>
+      <c r="D54" t="str">
+        <v>Cost of Sales</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55">
+        <v>2402</v>
+      </c>
+      <c r="B55" t="str">
+        <v>Uncategorised Expense</v>
+      </c>
+      <c r="C55" t="str">
+        <v>Expenses</v>
+      </c>
+      <c r="D55" t="str">
+        <v>Office/General Administrative Expenses</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56">
+        <v>2405</v>
+      </c>
+      <c r="B56" t="str">
+        <v>Accounting and bookkeeping</v>
+      </c>
+      <c r="C56" t="str">
+        <v>Expenses</v>
+      </c>
+      <c r="D56" t="str">
+        <v>Office/General Administrative Expenses</v>
+      </c>
+      <c r="E56" t="str">
+        <v>Professional fees charged to your business by an accountant or bookkeeper</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57">
+        <v>2406</v>
+      </c>
+      <c r="B57" t="str">
+        <v>Advertising and marketing</v>
+      </c>
+      <c r="C57" t="str">
+        <v>Expenses</v>
+      </c>
+      <c r="D57" t="str">
+        <v>Office/General Administrative Expenses</v>
+      </c>
+      <c r="E57" t="str">
+        <v>Fees and charges incurred by your business for advertising the goods and services it sells</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58">
+        <v>2407</v>
+      </c>
+      <c r="B58" t="str">
+        <v>Bank charges and fees</v>
+      </c>
+      <c r="C58" t="str">
+        <v>Expenses</v>
+      </c>
+      <c r="D58" t="str">
+        <v>Office/General Administrative Expenses</v>
+      </c>
+      <c r="E58" t="str">
+        <v>Fees charged by your bank for providing its services to your business</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59">
+        <v>2408</v>
+      </c>
+      <c r="B59" t="str">
+        <v>Gifts and donations</v>
+      </c>
+      <c r="C59" t="str">
+        <v>Expenses</v>
+      </c>
+      <c r="D59" t="str">
+        <v>Office/General Administrative Expenses</v>
+      </c>
+      <c r="E59" t="str">
+        <v>Money and gifts donated to charity</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60">
+        <v>2409</v>
+      </c>
+      <c r="B60" t="str">
+        <v>Subscriptions</v>
+      </c>
+      <c r="C60" t="str">
+        <v>Expenses</v>
+      </c>
+      <c r="D60" t="str">
+        <v>Office/General Administrative Expenses</v>
+      </c>
+      <c r="E60" t="str">
+        <v>Subscriptions to publications, professional memberships or products such as cloud software</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61">
+        <v>2410</v>
+      </c>
+      <c r="B61" t="str">
+        <v>Meals and entertainment</v>
+      </c>
+      <c r="C61" t="str">
+        <v>Expenses</v>
+      </c>
+      <c r="D61" t="str">
+        <v>Office/General Administrative Expenses</v>
+      </c>
+      <c r="E61" t="str">
+        <v>Expenses incurred when traveling for business purposes or entertaining a business client</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62">
+        <v>2411</v>
+      </c>
+      <c r="B62" t="str">
+        <v>Fuel &amp; oils</v>
+      </c>
+      <c r="C62" t="str">
+        <v>Expenses</v>
+      </c>
+      <c r="D62" t="str">
+        <v>Office/General Administrative Expenses</v>
+      </c>
+      <c r="E62" t="str">
+        <v>Cost of fuels and oils required for operating your business vehicles</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63">
+        <v>2412</v>
+      </c>
+      <c r="B63" t="str">
+        <v>Registration and insurance</v>
+      </c>
+      <c r="C63" t="str">
+        <v>Expenses</v>
+      </c>
+      <c r="D63" t="str">
+        <v>Office/General Administrative Expenses</v>
+      </c>
+      <c r="E63" t="str">
+        <v>Registration and insurance costs for company vehicles</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64">
+        <v>2413</v>
+      </c>
+      <c r="B64" t="str">
+        <v>Motor vehicle expenses</v>
+      </c>
+      <c r="C64" t="str">
+        <v>Expenses</v>
+      </c>
+      <c r="D64" t="str">
+        <v>Office/General Administrative Expenses</v>
+      </c>
+      <c r="E64" t="str">
+        <v>Expenses incurred running company vehicles</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65">
+        <v>2414</v>
+      </c>
+      <c r="B65" t="str">
+        <v>Insurance</v>
+      </c>
+      <c r="C65" t="str">
+        <v>Expenses</v>
+      </c>
+      <c r="D65" t="str">
+        <v>Office/General Administrative Expenses</v>
+      </c>
+      <c r="E65" t="str">
+        <v>Expenses incurred to insure business assets</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66">
+        <v>2415</v>
+      </c>
+      <c r="B66" t="str">
+        <v>Office expenses</v>
+      </c>
+      <c r="C66" t="str">
+        <v>Expenses</v>
+      </c>
+      <c r="D66" t="str">
+        <v>Office/General Administrative Expenses</v>
+      </c>
+      <c r="E66" t="str">
+        <v>Costs to maintain office space and equipment</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67">
+        <v>2416</v>
+      </c>
+      <c r="B67" t="str">
+        <v>Postage &amp; shipping</v>
+      </c>
+      <c r="C67" t="str">
+        <v>Expenses</v>
+      </c>
+      <c r="D67" t="str">
+        <v>Office/General Administrative Expenses</v>
+      </c>
+      <c r="E67" t="str">
+        <v>Cost of postage and shipping related to your business operations</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68">
+        <v>2417</v>
+      </c>
+      <c r="B68" t="str">
+        <v>Printing, stationery &amp; supplies</v>
+      </c>
+      <c r="C68" t="str">
+        <v>Expenses</v>
+      </c>
+      <c r="D68" t="str">
+        <v>Office/General Administrative Expenses</v>
+      </c>
+      <c r="E68" t="str">
+        <v>Cost of printing, stationery and supplies for office use</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69">
+        <v>2418</v>
+      </c>
+      <c r="B69" t="str">
+        <v>Repairs and maintenance</v>
+      </c>
+      <c r="C69" t="str">
+        <v>Expenses</v>
+      </c>
+      <c r="D69" t="str">
+        <v>Office/General Administrative Expenses</v>
+      </c>
+      <c r="E69" t="str">
+        <v>Expenses incurred repairing or maintaining business assets e.g. office equipment</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70">
+        <v>2419</v>
+      </c>
+      <c r="B70" t="str">
+        <v>Staff amenities</v>
+      </c>
+      <c r="C70" t="str">
+        <v>Expenses</v>
+      </c>
+      <c r="D70" t="str">
+        <v>Office/General Administrative Expenses</v>
+      </c>
+      <c r="E70" t="str">
+        <v>Staff refreshments e.g. tea, coffee and biscults</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71">
+        <v>2420</v>
+      </c>
+      <c r="B71" t="str">
+        <v>Telephone &amp; internet expenses</v>
+      </c>
+      <c r="C71" t="str">
+        <v>Expenses</v>
+      </c>
+      <c r="D71" t="str">
+        <v>Office/General Administrative Expenses</v>
+      </c>
+      <c r="E71" t="str">
+        <v>Phone calls and internet expenses associated with operating your business</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72">
+        <v>2421</v>
+      </c>
+      <c r="B72" t="str">
+        <v>Travel expenses</v>
+      </c>
+      <c r="C72" t="str">
+        <v>Expenses</v>
+      </c>
+      <c r="D72" t="str">
+        <v>Office/General Administrative Expenses</v>
+      </c>
+      <c r="E72" t="str">
+        <v>Expenses incurred when travelling for business</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73">
+        <v>2422</v>
+      </c>
+      <c r="B73" t="str">
+        <v>Gas and electricity</v>
+      </c>
+      <c r="C73" t="str">
+        <v>Expenses</v>
+      </c>
+      <c r="D73" t="str">
+        <v>Office/General Administrative Expenses</v>
+      </c>
+      <c r="E73" t="str">
+        <v>Expenses incurred for utilities such as lighting, powering or heating business premises</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74">
+        <v>2424</v>
+      </c>
+      <c r="B74" t="str">
+        <v>Interest expense</v>
+      </c>
+      <c r="C74" t="str">
+        <v>Expenses</v>
+      </c>
+      <c r="D74" t="str">
+        <v>Office/General Administrative Expenses</v>
+      </c>
+      <c r="E74" t="str">
+        <v>Interest payable on borrowings</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75">
+        <v>2427</v>
+      </c>
+      <c r="B75" t="str">
+        <v>Contractor Expenses (non salary)</v>
+      </c>
+      <c r="C75" t="str">
+        <v>Expenses</v>
+      </c>
+      <c r="D75" t="str">
+        <v>Office/General Administrative Expenses</v>
+      </c>
+      <c r="E75" t="str">
+        <v>Monies paid to a contractor (not an employee) for work they've completed</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76">
+        <v>2434</v>
+      </c>
+      <c r="B76" t="str">
+        <v>Salary and wages - staff</v>
+      </c>
+      <c r="C76" t="str">
+        <v>Expenses</v>
+      </c>
+      <c r="D76" t="str">
+        <v>Office/General Administrative Expenses</v>
+      </c>
+      <c r="E76" t="str">
+        <v>Salaries and wages paid to employees</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77">
+        <v>2435</v>
+      </c>
+      <c r="B77" t="str">
+        <v>Workcover expenses</v>
+      </c>
+      <c r="C77" t="str">
+        <v>Expenses</v>
+      </c>
+      <c r="D77" t="str">
+        <v>Office/General Administrative Expenses</v>
+      </c>
+      <c r="E77" t="str">
+        <v>Workcover is a compulsory and protects employees if injured on the job</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78">
+        <v>2439</v>
+      </c>
+      <c r="B78" t="str">
+        <v>Shipping, Freight, and Delivery Postage &amp; Handling</v>
+      </c>
+      <c r="C78" t="str">
+        <v>Expenses</v>
+      </c>
+      <c r="D78" t="str">
+        <v>Office/General Administrative Expenses</v>
+      </c>
+      <c r="E78" t="str">
+        <v>Shipping, Freight, and Delivery Postage &amp; Handling</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79">
+        <v>2444</v>
+      </c>
+      <c r="B79" t="str">
+        <v>Wages Expense</v>
+      </c>
+      <c r="C79" t="str">
+        <v>Expenses</v>
+      </c>
+      <c r="D79" t="str">
+        <v>Office/General Administrative Expenses</v>
+      </c>
+      <c r="E79" t="str">
+        <v>Default account for recorded wages and salaries expenses</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80">
+        <v>2447</v>
+      </c>
+      <c r="B80" t="str">
+        <v>Superannuation Expense</v>
+      </c>
+      <c r="C80" t="str">
+        <v>Expenses</v>
+      </c>
+      <c r="D80" t="str">
+        <v>Office/General Administrative Expenses</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81">
+        <v>2452</v>
+      </c>
+      <c r="B81" t="str">
+        <v>Client Gift</v>
+      </c>
+      <c r="C81" t="str">
+        <v>Expenses</v>
+      </c>
+      <c r="D81" t="str">
+        <v>Office/General Administrative Expenses</v>
+      </c>
+      <c r="E81" t="str">
+        <v>Client Birthday</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82">
+        <v>2456</v>
+      </c>
+      <c r="B82" t="str">
+        <v>Unapplied Cash Bill Payment Expense</v>
+      </c>
+      <c r="C82" t="str">
+        <v>Expenses</v>
+      </c>
+      <c r="D82" t="str">
+        <v>Office/General Administrative Expenses</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83">
+        <v>2459</v>
+      </c>
+      <c r="B83" t="str">
+        <v>Car</v>
+      </c>
+      <c r="C83" t="str">
+        <v>Expenses</v>
+      </c>
+      <c r="D83" t="str">
+        <v>Office/General Administrative Expenses</v>
+      </c>
+      <c r="E83" t="str">
+        <v>Insurance</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84">
+        <v>2464</v>
+      </c>
+      <c r="B84" t="str">
+        <v>BAS Expense</v>
+      </c>
+      <c r="C84" t="str">
+        <v>Expenses</v>
+      </c>
+      <c r="D84" t="str">
+        <v>Office/General Administrative Expenses</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85">
+        <v>2470</v>
+      </c>
+      <c r="B85" t="str">
+        <v>Workers Comp icare</v>
+      </c>
+      <c r="C85" t="str">
+        <v>Expenses</v>
+      </c>
+      <c r="D85" t="str">
+        <v>Office/General Administrative Expenses</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86">
+        <v>2471</v>
+      </c>
+      <c r="B86" t="str">
+        <v>Car Insurance</v>
+      </c>
+      <c r="C86" t="str">
+        <v>Expenses</v>
+      </c>
+      <c r="D86" t="str">
+        <v>Office/General Administrative Expenses</v>
+      </c>
+      <c r="E86" t="str">
+        <v>Car Insurance NRMA</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87">
+        <v>2472</v>
+      </c>
+      <c r="B87" t="str">
+        <v>Insurance Income Protection</v>
+      </c>
+      <c r="C87" t="str">
+        <v>Expenses</v>
+      </c>
+      <c r="D87" t="str">
+        <v>Office/General Administrative Expenses</v>
+      </c>
+      <c r="E87" t="str">
+        <v>Insurance Income Protection</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88">
+        <v>2473</v>
+      </c>
+      <c r="B88" t="str">
+        <v>Car Insurance Honda</v>
+      </c>
+      <c r="C88" t="str">
+        <v>Expenses</v>
+      </c>
+      <c r="D88" t="str">
+        <v>Office/General Administrative Expenses</v>
+      </c>
+      <c r="E88" t="str">
+        <v>Car Insurance Honda NRMA</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89">
+        <v>2474</v>
+      </c>
+      <c r="B89" t="str">
+        <v>NDIS Audit</v>
+      </c>
+      <c r="C89" t="str">
+        <v>Expenses</v>
+      </c>
+      <c r="D89" t="str">
+        <v>Office/General Administrative Expenses</v>
+      </c>
+      <c r="E89" t="str">
+        <v>NDIS Registration Audit</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90">
+        <v>2475</v>
+      </c>
+      <c r="B90" t="str">
+        <v>DJ Expenses</v>
+      </c>
+      <c r="C90" t="str">
+        <v>Expenses</v>
+      </c>
+      <c r="D90" t="str">
+        <v>Office/General Administrative Expenses</v>
+      </c>
+      <c r="E90" t="str">
+        <v>DJ Equipment</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91">
+        <v>2494</v>
+      </c>
+      <c r="B91" t="str">
+        <v>Admin Fee</v>
+      </c>
+      <c r="C91" t="str">
+        <v>Expenses</v>
+      </c>
+      <c r="D91" t="str">
+        <v>Office/General Administrative Expenses</v>
+      </c>
+      <c r="E91" t="str">
+        <v>Admin Fee</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92">
+        <v>2495</v>
+      </c>
+      <c r="B92" t="str">
+        <v>Purchases</v>
+      </c>
+      <c r="C92" t="str">
+        <v>Expenses</v>
+      </c>
+      <c r="D92" t="str">
+        <v>Office/General Administrative Expenses</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93">
+        <v>2496</v>
+      </c>
+      <c r="B93" t="str">
+        <v>Bad Debt</v>
+      </c>
+      <c r="C93" t="str">
+        <v>Expenses</v>
+      </c>
+      <c r="D93" t="str">
+        <v>Office/General Administrative Expenses</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94">
+        <v>2423</v>
+      </c>
+      <c r="B94" t="str">
+        <v>Interest income</v>
+      </c>
+      <c r="C94" t="str">
+        <v>Other income</v>
+      </c>
+      <c r="D94" t="str">
+        <v>Other Miscellaneous Income</v>
+      </c>
+      <c r="E94" t="str">
+        <v>Interest earned from savings accounts, deposits or other investments</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95">
+        <v>2445</v>
+      </c>
+      <c r="B95" t="str">
+        <v>Employee Expenses</v>
+      </c>
+      <c r="C95" t="str">
+        <v>Other expense</v>
+      </c>
+      <c r="D95" t="str">
+        <v>Other Expense</v>
+      </c>
+      <c r="E95" t="str">
+        <v>Default account for recorded employee expenses</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96">
+        <v>2460</v>
+      </c>
+      <c r="B96" t="str">
+        <v>Reconciliation Discrepancies</v>
+      </c>
+      <c r="C96" t="str">
+        <v>Other expense</v>
+      </c>
+      <c r="D96" t="str">
+        <v>Other Expense</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97">
+        <v>2462</v>
+      </c>
+      <c r="B97" t="str">
+        <v>BAS Roundoff Gain or Loss</v>
+      </c>
+      <c r="C97" t="str">
+        <v>Other expense</v>
+      </c>
+      <c r="D97" t="str">
+        <v>Other Expense</v>
+      </c>
+    </row>
+  </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E97"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>